<commit_message>
first iter bug fixed + 2 votes tables
</commit_message>
<xml_diff>
--- a/WebContent/notAPartOfTheProject/Check-List.xlsx
+++ b/WebContent/notAPartOfTheProject/Check-List.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="9630" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -175,8 +176,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +243,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -605,44 +611,6 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="13" name="Picture 12" descr="Kinjrykiq.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11235213750" y="5484243"/>
-          <a:ext cx="142875" cy="162087"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>16893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>178980</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="Kinjrykiq.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -933,6 +901,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -967,6 +936,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1142,245 +1112,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="64.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="27.75" customHeight="1">
+    <row r="4" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="29.25" customHeight="1">
+    <row r="10" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="23.25" customHeight="1">
+    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" customHeight="1">
+    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="38.25">
+    <row r="17" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="27" customHeight="1">
+    <row r="22" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18.75">
+    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="27" customHeight="1">
+    <row r="27" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75" customHeight="1">
+    <row r="28" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="66" customHeight="1">
+    <row r="31" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18.75">
+    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="25.5">
+    <row r="36" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="28.5" customHeight="1">
+    <row r="38" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="51">
+    <row r="39" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="38.25">
+    <row r="40" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="18.75">
+    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="38.25">
+    <row r="44" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="25.5">
+    <row r="45" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -1393,24 +1363,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "check list update"
This reverts commit e34b857abd628df437e6f90da3bf62bff69f9bbc.
</commit_message>
<xml_diff>
--- a/WebContent/notAPartOfTheProject/Check-List.xlsx
+++ b/WebContent/notAPartOfTheProject/Check-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14760" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14760" windowHeight="5055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1080,196 +1080,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11235213750" y="4179318"/>
-          <a:ext cx="142875" cy="162087"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>16893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>178980</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26" descr="Kinjrykiq.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11235213750" y="5484243"/>
-          <a:ext cx="142875" cy="162087"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>16893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>178980</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27" descr="Kinjrykiq.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11235213750" y="5484243"/>
-          <a:ext cx="142875" cy="162087"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>16893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>178980</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 28" descr="Kinjrykiq.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11235213750" y="5484243"/>
-          <a:ext cx="142875" cy="162087"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>16893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>178980</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29" descr="Kinjrykiq.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11235213750" y="5484243"/>
-          <a:ext cx="142875" cy="162087"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>16893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>178980</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30" descr="Kinjrykiq.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11235213750" y="5484243"/>
           <a:ext cx="142875" cy="162087"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1569,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>